<commit_message>
feat: Add data of A3 first floor.
</commit_message>
<xml_diff>
--- a/src/data/a3.xlsx
+++ b/src/data/a3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -64,7 +64,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Zhong Min Kitchen 
+      <t xml:space="preserve">Print Area
 </t>
     </r>
     <r>
@@ -72,28 +72,12 @@
         <sz val="10"/>
         <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">中闽美食</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">restaurant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zhongmin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bean's Express</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mad Plate Express</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mad</t>
+      </rPr>
+      <t xml:space="preserve">打印区</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">daily_necessity</t>
   </si>
   <si>
     <r>
@@ -103,119 +87,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Xiao Jiu Zho</t>
+      <t xml:space="preserve">MINI CINEMA
+</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">小九州</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Castle imn the sky 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">膳一城</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">castle</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Penang Flavour
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">槟城风味</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">penang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kami Cemerlang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kami</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Takwa Muslim Stir Fry 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">中国穆斯林小炒</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">takwa</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Uni Hotpot 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">有你香锅</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">hotpot</t>
+      </rPr>
+      <t xml:space="preserve">小影院</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">entertainment</t>
   </si>
   <si>
     <r>
@@ -255,6 +140,9 @@
       </rPr>
       <t xml:space="preserve">园</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
   </si>
   <si>
     <t xml:space="preserve">shiyuan</t>
@@ -488,7 +376,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -514,7 +402,6 @@
       <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -532,6 +419,12 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="LXGW WenKai Mono"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -639,7 +532,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,7 +669,7 @@
   </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
@@ -1462,10 +1355,10 @@
   </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1507,121 +1400,75 @@
       <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="n">
-        <v>9</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="A7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -2145,7 +1992,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B10 B19 B21:B1010" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B10 B19 B21:B1003" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2206,13 +2053,13 @@
     </row>
     <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>4</v>
@@ -2244,13 +2091,13 @@
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>4</v>
@@ -2289,13 +2136,13 @@
     </row>
     <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>2</v>
@@ -2327,13 +2174,13 @@
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F15" s="11" t="n">
         <f aca="false">TRUE()</f>
@@ -2342,13 +2189,13 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F16" s="11" t="n">
         <f aca="false">TRUE()</f>
@@ -2357,13 +2204,13 @@
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D17" s="9" t="n">
         <v>2</v>
@@ -2466,13 +2313,13 @@
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F31" s="11" t="n">
         <f aca="false">TRUE()</f>
@@ -2481,13 +2328,13 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F32" s="11" t="n">
         <f aca="false">TRUE()</f>
@@ -2496,13 +2343,13 @@
     </row>
     <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F33" s="11" t="n">
         <f aca="false">TRUE()</f>
@@ -2511,13 +2358,13 @@
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F34" s="11" t="n">
         <f aca="false">TRUE()</f>

</xml_diff>